<commit_message>
Updated Excel file to have same data names as in Schema
</commit_message>
<xml_diff>
--- a/DummyData/DummyData.xlsx
+++ b/DummyData/DummyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="150">
   <si>
     <t>name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Through The Loops</t>
   </si>
   <si>
-    <t>image-url</t>
-  </si>
-  <si>
     <t>Shawl</t>
   </si>
   <si>
@@ -426,6 +423,57 @@
   </si>
   <si>
     <t>730 - 1260</t>
+  </si>
+  <si>
+    <t>4, 6</t>
+  </si>
+  <si>
+    <t>3.5, 6.0</t>
+  </si>
+  <si>
+    <t>3, 2, 1</t>
+  </si>
+  <si>
+    <t>3.25, 2.75, 2.25</t>
+  </si>
+  <si>
+    <t>6, 5.5</t>
+  </si>
+  <si>
+    <t>10, 9</t>
+  </si>
+  <si>
+    <t>1 1/2, 2 1/2</t>
+  </si>
+  <si>
+    <t>2.5, 3.0</t>
+  </si>
+  <si>
+    <t>0, 1 1/2</t>
+  </si>
+  <si>
+    <t>2.0, 2.5</t>
+  </si>
+  <si>
+    <t>"4.0"</t>
+  </si>
+  <si>
+    <t>"5.0"</t>
+  </si>
+  <si>
+    <t>"3.0"</t>
+  </si>
+  <si>
+    <t>"9.0"</t>
+  </si>
+  <si>
+    <t>"6.0"</t>
+  </si>
+  <si>
+    <t>image1</t>
+  </si>
+  <si>
+    <t>image2</t>
   </si>
 </sst>
 </file>
@@ -777,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K29"/>
+  <dimension ref="A2:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -796,31 +844,31 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -831,31 +879,31 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -866,31 +914,31 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -898,34 +946,34 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -933,39 +981,39 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -973,8 +1021,8 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>4</v>
+      <c r="D7" t="s">
+        <v>133</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -988,328 +1036,439 @@
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
+      <c r="I7" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" t="s">
+        <v>138</v>
       </c>
       <c r="K7">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>4.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8">
+        <v>3.25</v>
+      </c>
+      <c r="F8">
+        <v>4.5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8">
+        <v>2.25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>136</v>
+      </c>
+      <c r="J8" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I9">
-        <v>1</v>
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9">
+        <v>437</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>609</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>4.5</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>3.5</v>
-      </c>
-      <c r="E10">
-        <v>3.25</v>
-      </c>
-      <c r="F10">
-        <v>4.5</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>2.25</v>
-      </c>
-      <c r="I10">
-        <v>3.25</v>
-      </c>
-      <c r="J10">
-        <v>6</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
+        <v>148</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="I11">
-        <v>2.75</v>
-      </c>
-      <c r="J11">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I12">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13">
-        <v>437</v>
-      </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13">
-        <v>609</v>
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" t="s">
-        <v>101</v>
-      </c>
-      <c r="K15" t="s">
-        <v>105</v>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="I18" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="J18" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" t="s">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>10.5</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" t="s">
-        <v>107</v>
+        <v>141</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
       </c>
       <c r="J19" t="s">
-        <v>112</v>
-      </c>
-      <c r="K19" t="s">
-        <v>116</v>
+        <v>139</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>3.75</v>
+      </c>
+      <c r="C20">
+        <v>3.5</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
-        <v>68</v>
+        <v>146</v>
+      </c>
+      <c r="G20">
+        <v>6.5</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="J20" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="K20" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" t="s">
-        <v>94</v>
+        <v>12</v>
+      </c>
+      <c r="I21">
+        <v>185</v>
       </c>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="K21" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
@@ -1330,204 +1489,51 @@
         <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="I22" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="J22" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="K22" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="F23">
-        <v>13</v>
-      </c>
-      <c r="G23">
-        <v>10.5</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>6</v>
-      </c>
-      <c r="J23">
-        <v>1.5</v>
-      </c>
-      <c r="K23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H24">
-        <v>1.5</v>
-      </c>
-      <c r="J24">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25">
-        <v>3.75</v>
-      </c>
-      <c r="C25">
-        <v>3.5</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <v>6</v>
-      </c>
-      <c r="F25">
-        <v>9</v>
-      </c>
-      <c r="G25">
-        <v>6.5</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>4</v>
-      </c>
-      <c r="J25">
-        <v>2.5</v>
-      </c>
-      <c r="K25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H26">
-        <v>2.5</v>
-      </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E27" t="s">
-        <v>129</v>
-      </c>
-      <c r="F27" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" t="s">
-        <v>131</v>
-      </c>
-      <c r="H27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27">
-        <v>185</v>
-      </c>
-      <c r="J27" t="s">
-        <v>132</v>
-      </c>
-      <c r="K27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D23" t="s">
         <v>51</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E23" t="s">
         <v>58</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F23" t="s">
         <v>64</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H23" t="s">
         <v>75</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I23" t="s">
         <v>109</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J23" t="s">
         <v>113</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K23" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" t="s">
-        <v>71</v>
-      </c>
-      <c r="H29" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" t="s">
-        <v>110</v>
-      </c>
-      <c r="J29" t="s">
-        <v>114</v>
-      </c>
-      <c r="K29" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more data to the sheet, modified the possible schema for multiple images. Updated index with all categories from sheet and fixed some minor bugs.
</commit_message>
<xml_diff>
--- a/DummyData/DummyData.xlsx
+++ b/DummyData/DummyData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\School\CSCI 344\Projects\FinalProject\DummyData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaitlin\Dropbox\University\CSCI 344\_Term Project\DummyData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="165">
   <si>
     <t>name</t>
   </si>
@@ -474,6 +474,51 @@
   </si>
   <si>
     <t>image2</t>
+  </si>
+  <si>
+    <t>Hiker's Waistcoat</t>
+  </si>
+  <si>
+    <t>The Fibre Company</t>
+  </si>
+  <si>
+    <t>Kelbourne Woollens</t>
+  </si>
+  <si>
+    <t>Vest</t>
+  </si>
+  <si>
+    <t>7, 8</t>
+  </si>
+  <si>
+    <t>4.5 - 5.0</t>
+  </si>
+  <si>
+    <t>700 - 900</t>
+  </si>
+  <si>
+    <t>http://images4-cdn.ravelrycache.com/uploads/FibreCompany/143369516/hikers2.jpg</t>
+  </si>
+  <si>
+    <t>https://images4-b.ravelrycache.com/uploads/FibreCompany/143369517/hikers1_medium2.jpg</t>
+  </si>
+  <si>
+    <t>Nordic Trail</t>
+  </si>
+  <si>
+    <t>Elizabeth Smith</t>
+  </si>
+  <si>
+    <t>The Brown Stitch</t>
+  </si>
+  <si>
+    <t>460 - 780</t>
+  </si>
+  <si>
+    <t>https://images4-e.ravelrycache.com/uploads/elizknits/142073883/Nordic-Trail_1_medium.jpg</t>
+  </si>
+  <si>
+    <t>https://images4-b.ravelrycache.com/uploads/elizknits/142073896/Nordic-Trail_2_medium.jpg</t>
   </si>
 </sst>
 </file>
@@ -518,9 +563,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -836,19 +887,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K23"/>
+  <dimension ref="A2:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.68359375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -882,8 +933,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -917,8 +968,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
@@ -952,8 +1003,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
@@ -987,8 +1038,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -1022,78 +1073,78 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>7</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>8</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>4.5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>3.25</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>4.5</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>2.25</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B9" t="s">
@@ -1127,8 +1178,8 @@
         <v>609</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1152,7 +1203,7 @@
       <c r="H10" t="s">
         <v>76</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="J10" t="s">
@@ -1162,8 +1213,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B11" t="s">
@@ -1187,7 +1238,7 @@
       <c r="H11" t="s">
         <v>77</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="J11" t="s">
@@ -1197,8 +1248,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B14" t="s">
@@ -1232,8 +1283,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
@@ -1267,8 +1318,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
@@ -1302,8 +1353,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
@@ -1337,8 +1388,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
@@ -1372,78 +1423,78 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>4</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>6</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>10</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>13</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>10.5</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="2">
         <v>6</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>3.75</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>3.5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>6.5</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B21" t="s">
@@ -1477,23 +1528,23 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G22" t="s">
@@ -1502,7 +1553,7 @@
       <c r="H22" t="s">
         <v>74</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
         <v>108</v>
       </c>
       <c r="J22" t="s">
@@ -1512,8 +1563,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B23" t="s">
@@ -1537,7 +1588,7 @@
       <c r="H23" t="s">
         <v>75</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="1" t="s">
         <v>109</v>
       </c>
       <c r="J23" t="s">
@@ -1545,13 +1596,131 @@
       </c>
       <c r="K23" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="I10" r:id="rId2"/>
+    <hyperlink ref="I22" r:id="rId3"/>
+    <hyperlink ref="I23" r:id="rId4"/>
+    <hyperlink ref="I11" r:id="rId5"/>
+    <hyperlink ref="C22" r:id="rId6"/>
+    <hyperlink ref="E22" r:id="rId7"/>
+    <hyperlink ref="F22" r:id="rId8"/>
+    <hyperlink ref="B33" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>